<commit_message>
Removed package grateful since it was buggy, fixed path for setrank results, re-run everything except setrank analysis
</commit_message>
<xml_diff>
--- a/R_output_files/Tables/Significant_Genes.xlsx
+++ b/R_output_files/Tables/Significant_Genes.xlsx
@@ -404,7 +404,7 @@
         <v>3.93100666757752</v>
       </c>
       <c r="D2">
-        <v>0.02353655029410975</v>
+        <v>0.02353655028574947</v>
       </c>
       <c r="E2">
         <v>0.0001500782840600025</v>
@@ -427,13 +427,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.6747870700246594</v>
+        <v>0.6747870700246759</v>
       </c>
       <c r="D3">
-        <v>0.0008689191171967279</v>
+        <v>0.0008689191171020561</v>
       </c>
       <c r="E3">
-        <v>3.68681836191609e-07</v>
+        <v>3.68681836142338e-07</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -453,13 +453,13 @@
         </is>
       </c>
       <c r="C4">
-        <v>-0.4100801103343778</v>
+        <v>-0.4100801103343769</v>
       </c>
       <c r="D4">
-        <v>0.03633971621978432</v>
+        <v>0.03633971622202494</v>
       </c>
       <c r="E4">
-        <v>0.00075978935322294</v>
+        <v>0.0007597893531850605</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -479,13 +479,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>-0.9370872899338127</v>
+        <v>-0.9370872899338029</v>
       </c>
       <c r="D5">
-        <v>0.005798527488223729</v>
+        <v>0.005798527488752711</v>
       </c>
       <c r="E5">
-        <v>1.754812029004559e-05</v>
+        <v>1.754812028981064e-05</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -505,13 +505,13 @@
         </is>
       </c>
       <c r="C6">
-        <v>-0.3102011649719719</v>
+        <v>-0.3102011649719746</v>
       </c>
       <c r="D6">
-        <v>0.03277896192965388</v>
+        <v>0.03277896193031708</v>
       </c>
       <c r="E6">
-        <v>0.0005883136654183764</v>
+        <v>0.0005883136653759474</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -531,13 +531,13 @@
         </is>
       </c>
       <c r="C7">
-        <v>-0.4236844197930345</v>
+        <v>-0.4236844197930337</v>
       </c>
       <c r="D7">
-        <v>0.04401564446407619</v>
+        <v>0.04401564446100836</v>
       </c>
       <c r="E7">
-        <v>0.001076319765016724</v>
+        <v>0.001076319765016491</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -557,13 +557,13 @@
         </is>
       </c>
       <c r="C8">
-        <v>-0.4055782818989194</v>
+        <v>-0.4055782818989165</v>
       </c>
       <c r="D8">
-        <v>0.03782848334181468</v>
+        <v>0.03782848333505309</v>
       </c>
       <c r="E8">
-        <v>0.0008389440474937139</v>
+        <v>0.0008389440474730952</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -583,13 +583,13 @@
         </is>
       </c>
       <c r="C9">
-        <v>-0.3359145435862986</v>
+        <v>-0.3359145435862904</v>
       </c>
       <c r="D9">
-        <v>0.004297799870456888</v>
+        <v>0.004297799870286504</v>
       </c>
       <c r="E9">
-        <v>2.421190451521512e-05</v>
+        <v>2.421190451206497e-05</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -609,13 +609,13 @@
         </is>
       </c>
       <c r="C10">
-        <v>-0.264812338664068</v>
+        <v>-0.26481233866407</v>
       </c>
       <c r="D10">
-        <v>0.02355970558724607</v>
+        <v>0.02355970558507242</v>
       </c>
       <c r="E10">
-        <v>0.0004337243188646175</v>
+        <v>0.0004337243188246013</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -635,13 +635,13 @@
         </is>
       </c>
       <c r="C11">
-        <v>-0.2786563266807706</v>
+        <v>-0.2786563266807685</v>
       </c>
       <c r="D11">
-        <v>0.04702885656926308</v>
+        <v>0.04702885656693807</v>
       </c>
       <c r="E11">
-        <v>0.001567363178648893</v>
+        <v>0.001567363178571405</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -661,13 +661,13 @@
         </is>
       </c>
       <c r="C12">
-        <v>-0.3778846426156856</v>
+        <v>-0.3778846426156852</v>
       </c>
       <c r="D12">
-        <v>0.03488258415377721</v>
+        <v>0.03488258414835176</v>
       </c>
       <c r="E12">
-        <v>0.0008569755734713054</v>
+        <v>0.0008569755734604944</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -687,13 +687,13 @@
         </is>
       </c>
       <c r="C13">
-        <v>-0.7100741567090137</v>
+        <v>-0.7100741567090152</v>
       </c>
       <c r="D13">
-        <v>0.0009196851532549835</v>
+        <v>0.0009196851533286504</v>
       </c>
       <c r="E13">
-        <v>2.124233465124073e-06</v>
+        <v>2.124233465171332e-06</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -713,13 +713,13 @@
         </is>
       </c>
       <c r="C14">
-        <v>-0.3203020860636872</v>
+        <v>-0.3203020860636837</v>
       </c>
       <c r="D14">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E14">
-        <v>0.0004785304394527461</v>
+        <v>0.0004785304394290875</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -739,13 +739,13 @@
         </is>
       </c>
       <c r="C15">
-        <v>-0.6136940551485045</v>
+        <v>-0.6136940551485035</v>
       </c>
       <c r="D15">
-        <v>2.133863964127449e-07</v>
+        <v>2.13386396379273e-07</v>
       </c>
       <c r="E15">
-        <v>5.03390650114535e-11</v>
+        <v>5.033906500499784e-11</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -765,13 +765,13 @@
         </is>
       </c>
       <c r="C16">
-        <v>-0.3725629689806041</v>
+        <v>-0.3725629689805971</v>
       </c>
       <c r="D16">
-        <v>0.04815621131565105</v>
+        <v>0.0481562113160796</v>
       </c>
       <c r="E16">
-        <v>0.001442871269877277</v>
+        <v>0.001442871269845052</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -791,13 +791,13 @@
         </is>
       </c>
       <c r="C17">
-        <v>-0.4761544188765726</v>
+        <v>-0.4761544188765746</v>
       </c>
       <c r="D17">
-        <v>0.0003654438157607383</v>
+        <v>0.0003654438157074427</v>
       </c>
       <c r="E17">
-        <v>3.175314022205486e-07</v>
+        <v>3.175314021963032e-07</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -817,13 +817,13 @@
         </is>
       </c>
       <c r="C18">
-        <v>0.4790995488285074</v>
+        <v>0.4790995488285024</v>
       </c>
       <c r="D18">
-        <v>0.01902096648372071</v>
+        <v>0.01902096648427938</v>
       </c>
       <c r="E18">
-        <v>0.0002223806554434159</v>
+        <v>0.0002223806554372456</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -843,13 +843,13 @@
         </is>
       </c>
       <c r="C19">
-        <v>-0.7785598149513288</v>
+        <v>-0.7785598149513252</v>
       </c>
       <c r="D19">
-        <v>0.009307550149730047</v>
+        <v>0.009307550149278174</v>
       </c>
       <c r="E19">
-        <v>3.213449382590545e-05</v>
+        <v>3.213449382325824e-05</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -869,13 +869,13 @@
         </is>
       </c>
       <c r="C20">
-        <v>-0.3882599464528861</v>
+        <v>-0.3882599464528769</v>
       </c>
       <c r="D20">
-        <v>0.009366550973321522</v>
+        <v>0.00936655097171786</v>
       </c>
       <c r="E20">
-        <v>6.712797809380426e-05</v>
+        <v>6.712797808766388e-05</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -895,13 +895,13 @@
         </is>
       </c>
       <c r="C21">
-        <v>5.169713885372582</v>
+        <v>5.169713885372581</v>
       </c>
       <c r="D21">
-        <v>0.002009219655518218</v>
+        <v>0.002009219655624703</v>
       </c>
       <c r="E21">
-        <v>6.32007979208613e-06</v>
+        <v>6.320079792086236e-06</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -921,13 +921,13 @@
         </is>
       </c>
       <c r="C22">
-        <v>4.950718050006491</v>
+        <v>4.950718050006484</v>
       </c>
       <c r="D22">
-        <v>0.0009196851532549835</v>
+        <v>0.0009196851533286504</v>
       </c>
       <c r="E22">
-        <v>1.682060026593432e-06</v>
+        <v>1.682060026593491e-06</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -947,13 +947,13 @@
         </is>
       </c>
       <c r="C23">
-        <v>-0.3045465579884744</v>
+        <v>-0.3045465579884745</v>
       </c>
       <c r="D23">
-        <v>0.03277896192965388</v>
+        <v>0.03277896193031708</v>
       </c>
       <c r="E23">
-        <v>0.0007284979230740125</v>
+        <v>0.0007284979230322336</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -973,13 +973,13 @@
         </is>
       </c>
       <c r="C24">
-        <v>-0.7277222812200356</v>
+        <v>-0.727722281220033</v>
       </c>
       <c r="D24">
-        <v>1.894832370497952e-12</v>
+        <v>1.894832369961831e-12</v>
       </c>
       <c r="E24">
-        <v>3.007161280361981e-16</v>
+        <v>3.007161279511137e-16</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -999,13 +999,13 @@
         </is>
       </c>
       <c r="C25">
-        <v>-0.4114188685873616</v>
+        <v>-0.4114188685873482</v>
       </c>
       <c r="D25">
-        <v>0.04316546773061721</v>
+        <v>0.04316546773187632</v>
       </c>
       <c r="E25">
-        <v>0.0009743480366762875</v>
+        <v>0.0009743480366490565</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1025,13 +1025,13 @@
         </is>
       </c>
       <c r="C26">
-        <v>-0.3174481279190333</v>
+        <v>-0.3174481279190322</v>
       </c>
       <c r="D26">
-        <v>0.009366550973321522</v>
+        <v>0.00936655097171786</v>
       </c>
       <c r="E26">
-        <v>7.324673568504545e-05</v>
+        <v>7.324673567759412e-05</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1051,13 +1051,13 @@
         </is>
       </c>
       <c r="C27">
-        <v>-0.3068420233685946</v>
+        <v>-0.3068420233685891</v>
       </c>
       <c r="D27">
-        <v>0.03474960898520096</v>
+        <v>0.03474960898356001</v>
       </c>
       <c r="E27">
-        <v>0.0007976894643404542</v>
+        <v>0.0007976894643009584</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1077,13 +1077,13 @@
         </is>
       </c>
       <c r="C28">
-        <v>-0.5500662371387024</v>
+        <v>-0.5500662371387026</v>
       </c>
       <c r="D28">
-        <v>0.03277896192965388</v>
+        <v>0.03277896193031708</v>
       </c>
       <c r="E28">
-        <v>0.0006144450795774059</v>
+        <v>0.0006144450795861513</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1103,13 +1103,13 @@
         </is>
       </c>
       <c r="C29">
-        <v>0.5355406741566102</v>
+        <v>0.5355406741566427</v>
       </c>
       <c r="D29">
-        <v>0.03900016812707151</v>
+        <v>0.03900016812931886</v>
       </c>
       <c r="E29">
-        <v>0.0002420910500040695</v>
+        <v>0.000242091049986705</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1129,13 +1129,13 @@
         </is>
       </c>
       <c r="C30">
-        <v>-0.4520760132200052</v>
+        <v>-0.452076013220005</v>
       </c>
       <c r="D30">
-        <v>0.02514286284877378</v>
+        <v>0.02514286284711378</v>
       </c>
       <c r="E30">
-        <v>0.0003856186263764394</v>
+        <v>0.0003856186263744367</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1155,13 +1155,13 @@
         </is>
       </c>
       <c r="C31">
-        <v>-0.250677105639354</v>
+        <v>-0.2506771056393415</v>
       </c>
       <c r="D31">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E31">
-        <v>0.0005876015617194645</v>
+        <v>0.0005876015616572124</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1181,13 +1181,13 @@
         </is>
       </c>
       <c r="C32">
-        <v>-0.4271431255388159</v>
+        <v>-0.4271431255388091</v>
       </c>
       <c r="D32">
-        <v>0.002329153828291241</v>
+        <v>0.002329153828131321</v>
       </c>
       <c r="E32">
-        <v>1.071968677585478e-05</v>
+        <v>1.071968677511876e-05</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1207,13 +1207,13 @@
         </is>
       </c>
       <c r="C33">
-        <v>1.743861683319534</v>
+        <v>1.743861683319559</v>
       </c>
       <c r="D33">
-        <v>0.0009196851532549835</v>
+        <v>0.0009196851533286504</v>
       </c>
       <c r="E33">
-        <v>6.670326023058541e-07</v>
+        <v>6.670326023530225e-07</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1233,13 +1233,13 @@
         </is>
       </c>
       <c r="C34">
-        <v>0.3717166871213363</v>
+        <v>0.3717166871213342</v>
       </c>
       <c r="D34">
-        <v>0.03567620661390576</v>
+        <v>0.03567620661063373</v>
       </c>
       <c r="E34">
-        <v>0.0007586805147061958</v>
+        <v>0.0007586805146827637</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1259,13 +1259,13 @@
         </is>
       </c>
       <c r="C35">
-        <v>-0.4796261666086752</v>
+        <v>-0.4796261666086732</v>
       </c>
       <c r="D35">
-        <v>0.000544958633238181</v>
+        <v>0.0005449586332023876</v>
       </c>
       <c r="E35">
-        <v>6.971099389558175e-07</v>
+        <v>6.971099389079853e-07</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1285,13 +1285,13 @@
         </is>
       </c>
       <c r="C36">
-        <v>-0.3334593595642121</v>
+        <v>-0.3334593595642086</v>
       </c>
       <c r="D36">
-        <v>0.03095961807739343</v>
+        <v>0.03095961807618118</v>
       </c>
       <c r="E36">
-        <v>0.0006780482608257273</v>
+        <v>0.0006780482607991772</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1311,13 +1311,13 @@
         </is>
       </c>
       <c r="C37">
-        <v>-0.2763555813100579</v>
+        <v>-0.2763555813100557</v>
       </c>
       <c r="D37">
-        <v>0.0009145016978814393</v>
+        <v>0.0009145016975501846</v>
       </c>
       <c r="E37">
-        <v>1.650094692300282e-06</v>
+        <v>1.650094691802951e-06</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1337,13 +1337,13 @@
         </is>
       </c>
       <c r="C38">
-        <v>-0.4053128573475663</v>
+        <v>-0.4053128573475651</v>
       </c>
       <c r="D38">
-        <v>0.0195286484946758</v>
+        <v>0.01952864849493564</v>
       </c>
       <c r="E38">
-        <v>0.0002306332351247112</v>
+        <v>0.0002306332351118909</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1363,13 +1363,13 @@
         </is>
       </c>
       <c r="C39">
-        <v>0.9612395587293076</v>
+        <v>0.9612395587292608</v>
       </c>
       <c r="D39">
-        <v>0.03477815041019694</v>
+        <v>0.03477815040807382</v>
       </c>
       <c r="E39">
-        <v>0.000182895791189711</v>
+        <v>0.0001828957911828147</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1392,7 +1392,7 @@
         <v>-4.402773048584629</v>
       </c>
       <c r="D40">
-        <v>0.01791268932939229</v>
+        <v>0.01791268933046622</v>
       </c>
       <c r="E40">
         <v>0.0002155998747174022</v>
@@ -1418,10 +1418,10 @@
         <v>-2.915742770200414</v>
       </c>
       <c r="D41">
-        <v>0.02606818192166425</v>
+        <v>0.02606818192427626</v>
       </c>
       <c r="E41">
-        <v>1.416393669861458e-05</v>
+        <v>1.416393669862964e-05</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1441,13 +1441,13 @@
         </is>
       </c>
       <c r="C42">
-        <v>-0.3945204111180869</v>
+        <v>-0.3945204111180888</v>
       </c>
       <c r="D42">
-        <v>0.0001605215024246578</v>
+        <v>0.0001605215023872253</v>
       </c>
       <c r="E42">
-        <v>1.034426257040205e-07</v>
+        <v>1.034426256861907e-07</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1467,13 +1467,13 @@
         </is>
       </c>
       <c r="C43">
-        <v>0.6227466474484251</v>
+        <v>0.6227466474484269</v>
       </c>
       <c r="D43">
-        <v>0.03900016812707151</v>
+        <v>0.03900016812931886</v>
       </c>
       <c r="E43">
-        <v>0.0008681726448361234</v>
+        <v>0.000868172644840154</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1493,13 +1493,13 @@
         </is>
       </c>
       <c r="C44">
-        <v>1.184745208135278</v>
+        <v>1.184745208135277</v>
       </c>
       <c r="D44">
-        <v>0.0009145016978814393</v>
+        <v>0.0009145016975501846</v>
       </c>
       <c r="E44">
-        <v>1.384648830142916e-06</v>
+        <v>1.384648830229814e-06</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1519,13 +1519,13 @@
         </is>
       </c>
       <c r="C45">
-        <v>0.764370144184797</v>
+        <v>0.7643701441847989</v>
       </c>
       <c r="D45">
-        <v>0.04803781146799448</v>
+        <v>0.04803781147387492</v>
       </c>
       <c r="E45">
-        <v>0.001550601194837413</v>
+        <v>0.001550601194886954</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -1545,13 +1545,13 @@
         </is>
       </c>
       <c r="C46">
-        <v>-0.3786588083243145</v>
+        <v>-0.3786588083243169</v>
       </c>
       <c r="D46">
-        <v>0.001967306587449872</v>
+        <v>0.001967306587172481</v>
       </c>
       <c r="E46">
-        <v>5.337136398951936e-06</v>
+        <v>5.337136398352135e-06</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -1571,13 +1571,13 @@
         </is>
       </c>
       <c r="C47">
-        <v>1.636845627770697</v>
+        <v>1.636845627770704</v>
       </c>
       <c r="D47">
-        <v>0.004811107791125669</v>
+        <v>0.004811107791943029</v>
       </c>
       <c r="E47">
-        <v>6.899414340945494e-06</v>
+        <v>6.899414341317873e-06</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -1597,13 +1597,13 @@
         </is>
       </c>
       <c r="C48">
-        <v>0.8173454170771214</v>
+        <v>0.8173454170771249</v>
       </c>
       <c r="D48">
-        <v>0.0331581219298428</v>
+        <v>0.03315812193287432</v>
       </c>
       <c r="E48">
-        <v>0.0005967900251654361</v>
+        <v>0.0005967900251789717</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -1623,13 +1623,13 @@
         </is>
       </c>
       <c r="C49">
-        <v>-0.3208083128595717</v>
+        <v>-0.3208083128595725</v>
       </c>
       <c r="D49">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E49">
-        <v>0.0005154592885033059</v>
+        <v>0.0005154592884715658</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -1649,13 +1649,13 @@
         </is>
       </c>
       <c r="C50">
-        <v>0.316866221126514</v>
+        <v>0.3168662211265153</v>
       </c>
       <c r="D50">
-        <v>0.04743949791216315</v>
+        <v>0.0474394979072087</v>
       </c>
       <c r="E50">
-        <v>0.001290086571668067</v>
+        <v>0.001290086571611809</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -1675,13 +1675,13 @@
         </is>
       </c>
       <c r="C51">
-        <v>-0.3868067495883707</v>
+        <v>-0.3868067495883742</v>
       </c>
       <c r="D51">
-        <v>0.01551411003660736</v>
+        <v>0.01551411003630156</v>
       </c>
       <c r="E51">
-        <v>0.0001562388997289095</v>
+        <v>0.0001562388997169059</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -1701,13 +1701,13 @@
         </is>
       </c>
       <c r="C52">
-        <v>-0.2798202764637773</v>
+        <v>-0.2798202764637761</v>
       </c>
       <c r="D52">
-        <v>0.04257024761234196</v>
+        <v>0.04257024760715106</v>
       </c>
       <c r="E52">
-        <v>0.001025122888875854</v>
+        <v>0.001025122888822081</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -1727,13 +1727,13 @@
         </is>
       </c>
       <c r="C53">
-        <v>-0.4504025519597262</v>
+        <v>-0.4504025519597205</v>
       </c>
       <c r="D53">
-        <v>0.01506999081389644</v>
+        <v>0.01506999081437997</v>
       </c>
       <c r="E53">
-        <v>0.0001586918783062355</v>
+        <v>0.0001586918783027542</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -1753,13 +1753,13 @@
         </is>
       </c>
       <c r="C54">
-        <v>-0.3772447293654116</v>
+        <v>-0.3772447293654105</v>
       </c>
       <c r="D54">
-        <v>0.02211292208551394</v>
+        <v>0.02211292208199917</v>
       </c>
       <c r="E54">
-        <v>0.0003739967059401013</v>
+        <v>0.0003739967059317679</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -1779,13 +1779,13 @@
         </is>
       </c>
       <c r="C55">
-        <v>0.5766279577967047</v>
+        <v>0.5766279577967051</v>
       </c>
       <c r="D55">
-        <v>0.04580293991767476</v>
+        <v>0.04580293991243103</v>
       </c>
       <c r="E55">
-        <v>0.001181930083231063</v>
+        <v>0.001181930083237119</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -1805,13 +1805,13 @@
         </is>
       </c>
       <c r="C56">
-        <v>-0.2664775512079839</v>
+        <v>-0.2664775512079682</v>
       </c>
       <c r="D56">
-        <v>0.04412449928642177</v>
+        <v>0.04412449928013371</v>
       </c>
       <c r="E56">
-        <v>0.001089935732842947</v>
+        <v>0.001089935732763355</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -1831,13 +1831,13 @@
         </is>
       </c>
       <c r="C57">
-        <v>-0.3544116078903296</v>
+        <v>-0.3544116078903323</v>
       </c>
       <c r="D57">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E57">
-        <v>0.0006285798191075875</v>
+        <v>0.0006285798190916134</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -1860,7 +1860,7 @@
         <v>2.819176062041834</v>
       </c>
       <c r="D58">
-        <v>0.01691257625866199</v>
+        <v>0.01691257625955805</v>
       </c>
       <c r="E58">
         <v>0.0001882432405628933</v>
@@ -1883,13 +1883,13 @@
         </is>
       </c>
       <c r="C59">
-        <v>0.4186480873016133</v>
+        <v>0.4186480873016145</v>
       </c>
       <c r="D59">
-        <v>0.03531868810357744</v>
+        <v>0.03531868810482049</v>
       </c>
       <c r="E59">
-        <v>0.0006664003550379949</v>
+        <v>0.0006664003550233861</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -1909,13 +1909,13 @@
         </is>
       </c>
       <c r="C60">
-        <v>3.963083262548574</v>
+        <v>3.963083262548573</v>
       </c>
       <c r="D60">
-        <v>0.01444076571208121</v>
+        <v>0.01444076571243776</v>
       </c>
       <c r="E60">
-        <v>4.456151149273746e-05</v>
+        <v>4.456151149273763e-05</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -1935,13 +1935,13 @@
         </is>
       </c>
       <c r="C61">
-        <v>0.8946948549623315</v>
+        <v>0.8946948549623355</v>
       </c>
       <c r="D61">
-        <v>0.01506999081389644</v>
+        <v>0.01506999081437997</v>
       </c>
       <c r="E61">
-        <v>0.0001584341904160442</v>
+        <v>0.0001584341904232501</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -1961,13 +1961,13 @@
         </is>
       </c>
       <c r="C62">
-        <v>0.4125666925108856</v>
+        <v>0.4125666925108648</v>
       </c>
       <c r="D62">
-        <v>0.03782848334181468</v>
+        <v>0.03782848333505309</v>
       </c>
       <c r="E62">
-        <v>0.0008212074544121502</v>
+        <v>0.0008212074543663963</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>3.794775234367701</v>
       </c>
       <c r="D63">
-        <v>0.03550524066706588</v>
+        <v>0.03550524067003014</v>
       </c>
       <c r="E63">
         <v>0.0001977611279535077</v>
@@ -2013,13 +2013,13 @@
         </is>
       </c>
       <c r="C64">
-        <v>-0.2562178795696496</v>
+        <v>-0.2562178795696465</v>
       </c>
       <c r="D64">
-        <v>0.03633971621978432</v>
+        <v>0.03633971622202494</v>
       </c>
       <c r="E64">
-        <v>0.0009429989480507443</v>
+        <v>0.0009429989479887449</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -2042,7 +2042,7 @@
         <v>-3.23940792737788</v>
       </c>
       <c r="D65">
-        <v>0.03900016812707151</v>
+        <v>0.03900016812931886</v>
       </c>
       <c r="E65">
         <v>0.001138029626257928</v>
@@ -2068,10 +2068,10 @@
         <v>2.762792984882858</v>
       </c>
       <c r="D66">
-        <v>0.01506999081389644</v>
+        <v>0.01506999081437997</v>
       </c>
       <c r="E66">
-        <v>0.0001401348296166788</v>
+        <v>0.0001401348296166783</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -2094,7 +2094,7 @@
         <v>3.152445412196216</v>
       </c>
       <c r="D67">
-        <v>0.005055948716604181</v>
+        <v>0.005055948716836424</v>
       </c>
       <c r="E67">
         <v>2.652006172924681e-05</v>
@@ -2117,13 +2117,13 @@
         </is>
       </c>
       <c r="C68">
-        <v>0.4103229934610363</v>
+        <v>0.4103229934610329</v>
       </c>
       <c r="D68">
-        <v>0.03633971621978432</v>
+        <v>0.03633971622202494</v>
       </c>
       <c r="E68">
-        <v>0.0007103873087658534</v>
+        <v>0.0007103873087476642</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -2143,13 +2143,13 @@
         </is>
       </c>
       <c r="C69">
-        <v>-0.4802159970439589</v>
+        <v>-0.4802159970439298</v>
       </c>
       <c r="D69">
-        <v>0.02514286284877378</v>
+        <v>0.02514286284711378</v>
       </c>
       <c r="E69">
-        <v>0.0003702185330213464</v>
+        <v>0.0003702185330047473</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -2169,13 +2169,13 @@
         </is>
       </c>
       <c r="C70">
-        <v>-0.4289970041593349</v>
+        <v>-0.4289970041593331</v>
       </c>
       <c r="D70">
-        <v>0.03096086714316363</v>
+        <v>0.03096086714413064</v>
       </c>
       <c r="E70">
-        <v>0.0006841419889112227</v>
+        <v>0.000684141988905824</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -2195,13 +2195,13 @@
         </is>
       </c>
       <c r="C71">
-        <v>-0.4183411881698608</v>
+        <v>-0.4183411881698596</v>
       </c>
       <c r="D71">
-        <v>0.005625838982361868</v>
+        <v>0.005625838981755759</v>
       </c>
       <c r="E71">
-        <v>3.552873081715371e-05</v>
+        <v>3.552873081548714e-05</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -2221,13 +2221,13 @@
         </is>
       </c>
       <c r="C72">
-        <v>0.3154735300697032</v>
+        <v>0.3154735300697107</v>
       </c>
       <c r="D72">
-        <v>0.002534037487511161</v>
+        <v>0.002534037487085139</v>
       </c>
       <c r="E72">
-        <v>7.322696441911808e-06</v>
+        <v>7.32269644053256e-06</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -2247,13 +2247,13 @@
         </is>
       </c>
       <c r="C73">
-        <v>-0.2734748506297343</v>
+        <v>-0.2734748506297415</v>
       </c>
       <c r="D73">
-        <v>0.004592942540983284</v>
+        <v>0.004592942540438952</v>
       </c>
       <c r="E73">
-        <v>2.778807084565666e-05</v>
+        <v>2.778807084053035e-05</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -2273,13 +2273,13 @@
         </is>
       </c>
       <c r="C74">
-        <v>-0.342231562263627</v>
+        <v>-0.3422315622636325</v>
       </c>
       <c r="D74">
-        <v>0.04492372637610642</v>
+        <v>0.0449237263759867</v>
       </c>
       <c r="E74">
-        <v>0.0009687578935666557</v>
+        <v>0.0009687578935168062</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -2302,7 +2302,7 @@
         <v>2.608403847115865</v>
       </c>
       <c r="D75">
-        <v>0.03277896192965388</v>
+        <v>0.03277896193031708</v>
       </c>
       <c r="E75">
         <v>0.0004067495960720987</v>
@@ -2325,13 +2325,13 @@
         </is>
       </c>
       <c r="C76">
-        <v>-0.5185636075043079</v>
+        <v>-0.5185636075043071</v>
       </c>
       <c r="D76">
-        <v>0.04381181348544171</v>
+        <v>0.04381181348333437</v>
       </c>
       <c r="E76">
-        <v>0.001106734929894572</v>
+        <v>0.00110673492990866</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -2351,13 +2351,13 @@
         </is>
       </c>
       <c r="C77">
-        <v>3.431683799039828</v>
+        <v>3.431683799039825</v>
       </c>
       <c r="D77">
-        <v>0.009409867498996999</v>
+        <v>0.009409867499495694</v>
       </c>
       <c r="E77">
-        <v>7.399777478694855e-05</v>
+        <v>7.399777478694968e-05</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -2377,13 +2377,13 @@
         </is>
       </c>
       <c r="C78">
-        <v>0.3736441300611167</v>
+        <v>0.3736441300611064</v>
       </c>
       <c r="D78">
-        <v>0.009366550973321522</v>
+        <v>0.00936655097171786</v>
       </c>
       <c r="E78">
-        <v>6.823435598917837e-05</v>
+        <v>6.823435598330759e-05</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -2403,13 +2403,13 @@
         </is>
       </c>
       <c r="C79">
-        <v>-0.5557725679080412</v>
+        <v>-0.5557725679080397</v>
       </c>
       <c r="D79">
-        <v>0.03633971621978432</v>
+        <v>0.03633971622202494</v>
       </c>
       <c r="E79">
-        <v>0.0004347935646750985</v>
+        <v>0.0004347935646722521</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -2429,13 +2429,13 @@
         </is>
       </c>
       <c r="C80">
-        <v>-0.245672798405272</v>
+        <v>-0.2456727984052799</v>
       </c>
       <c r="D80">
-        <v>0.03477815041019694</v>
+        <v>0.03477815040807382</v>
       </c>
       <c r="E80">
-        <v>0.0004671257402723735</v>
+        <v>0.000467125740219835</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -2455,13 +2455,13 @@
         </is>
       </c>
       <c r="C81">
-        <v>2.977766531879114</v>
+        <v>2.977766531879117</v>
       </c>
       <c r="D81">
-        <v>0.01741509362642408</v>
+        <v>0.0174150936232065</v>
       </c>
       <c r="E81">
-        <v>0.0001978302693632293</v>
+        <v>0.0001978302693632289</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -2481,13 +2481,13 @@
         </is>
       </c>
       <c r="C82">
-        <v>-0.41523879526762</v>
+        <v>-0.4152387952676207</v>
       </c>
       <c r="D82">
-        <v>0.02606818192166425</v>
+        <v>0.02606818192427626</v>
       </c>
       <c r="E82">
-        <v>0.0005061929637323294</v>
+        <v>0.0005061929637282059</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -2507,13 +2507,13 @@
         </is>
       </c>
       <c r="C83">
-        <v>-0.3122282208929509</v>
+        <v>-0.3122282208929488</v>
       </c>
       <c r="D83">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E83">
-        <v>0.0007657962278272162</v>
+        <v>0.0007657962277767953</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -2533,13 +2533,13 @@
         </is>
       </c>
       <c r="C84">
-        <v>-2.157875401550114</v>
+        <v>-2.157875401550134</v>
       </c>
       <c r="D84">
-        <v>0.00470179753198625</v>
+        <v>0.004701797531078375</v>
       </c>
       <c r="E84">
-        <v>8.552633886768402e-06</v>
+        <v>8.552633887176683e-06</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -2559,13 +2559,13 @@
         </is>
       </c>
       <c r="C85">
-        <v>3.13737912013</v>
+        <v>3.137379120129999</v>
       </c>
       <c r="D85">
-        <v>0.009365241640226642</v>
+        <v>0.009365241641312052</v>
       </c>
       <c r="E85">
-        <v>1.800882850766953e-05</v>
+        <v>1.800882850766917e-05</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -2585,13 +2585,13 @@
         </is>
       </c>
       <c r="C86">
-        <v>1.14332714150095</v>
+        <v>1.143327141501091</v>
       </c>
       <c r="D86">
-        <v>0.03474960898520096</v>
+        <v>0.03474960898356001</v>
       </c>
       <c r="E86">
-        <v>0.000175385294078474</v>
+        <v>0.0001753852940618136</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -2611,13 +2611,13 @@
         </is>
       </c>
       <c r="C87">
-        <v>-0.4002077741105518</v>
+        <v>-0.4002077741105503</v>
       </c>
       <c r="D87">
-        <v>0.008779509299463266</v>
+        <v>0.008779509299270207</v>
       </c>
       <c r="E87">
-        <v>5.955965961982339e-05</v>
+        <v>5.955965961732955e-05</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -2637,13 +2637,13 @@
         </is>
       </c>
       <c r="C88">
-        <v>1.201234812304025</v>
+        <v>1.201234812304031</v>
       </c>
       <c r="D88">
-        <v>0.03522641240978767</v>
+        <v>0.03522641241103029</v>
       </c>
       <c r="E88">
-        <v>0.0002464591178284332</v>
+        <v>0.0002464591178344786</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -2663,13 +2663,13 @@
         </is>
       </c>
       <c r="C89">
-        <v>-0.3225514272635629</v>
+        <v>-0.3225514272635577</v>
       </c>
       <c r="D89">
-        <v>0.04156990062851939</v>
+        <v>0.04156990062617836</v>
       </c>
       <c r="E89">
-        <v>0.0009271808559344743</v>
+        <v>0.0009271808559057228</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -2689,13 +2689,13 @@
         </is>
       </c>
       <c r="C90">
-        <v>-0.6448876137881963</v>
+        <v>-0.6448876137881978</v>
       </c>
       <c r="D90">
-        <v>0.001991359961106865</v>
+        <v>0.001991359961149462</v>
       </c>
       <c r="E90">
-        <v>4.062001610045331e-06</v>
+        <v>4.062001610050033e-06</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -2715,13 +2715,13 @@
         </is>
       </c>
       <c r="C91">
-        <v>-0.3521921377677794</v>
+        <v>-0.3521921377677792</v>
       </c>
       <c r="D91">
-        <v>0.02289688514022564</v>
+        <v>0.02289688513790355</v>
       </c>
       <c r="E91">
-        <v>0.0003154767866970381</v>
+        <v>0.000315476786686964</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -2741,13 +2741,13 @@
         </is>
       </c>
       <c r="C92">
-        <v>-0.329274605684512</v>
+        <v>-0.3292746056845092</v>
       </c>
       <c r="D92">
-        <v>0.009981144849153484</v>
+        <v>0.009981144848533874</v>
       </c>
       <c r="E92">
-        <v>9.968604775909466e-05</v>
+        <v>9.968604774979282e-05</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -2767,13 +2767,13 @@
         </is>
       </c>
       <c r="C93">
-        <v>0.7404154891407395</v>
+        <v>0.7404154891407385</v>
       </c>
       <c r="D93">
-        <v>0.005798527488223729</v>
+        <v>0.005798527488752711</v>
       </c>
       <c r="E93">
-        <v>4.549161035586133e-05</v>
+        <v>4.54916103575194e-05</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -2796,7 +2796,7 @@
         <v>1.858188748004513</v>
       </c>
       <c r="D94">
-        <v>0.03096086714316363</v>
+        <v>0.03096086714413064</v>
       </c>
       <c r="E94">
         <v>0.0006097289592029361</v>
@@ -2819,13 +2819,13 @@
         </is>
       </c>
       <c r="C95">
-        <v>5.050350004744045</v>
+        <v>5.050350004744043</v>
       </c>
       <c r="D95">
-        <v>0.002329153828291241</v>
+        <v>0.002329153828131321</v>
       </c>
       <c r="E95">
-        <v>1.232468183314835e-05</v>
+        <v>1.23246818331484e-05</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -2845,13 +2845,13 @@
         </is>
       </c>
       <c r="C96">
-        <v>-0.4362669287304904</v>
+        <v>-0.4362669287304911</v>
       </c>
       <c r="D96">
-        <v>0.0001818710940015185</v>
+        <v>0.0001818710939633201</v>
       </c>
       <c r="E96">
-        <v>1.35451230244449e-07</v>
+        <v>1.354512302254116e-07</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -2871,13 +2871,13 @@
         </is>
       </c>
       <c r="C97">
-        <v>-4.566552261618233</v>
+        <v>-4.566552261618236</v>
       </c>
       <c r="D97">
-        <v>0.04632659953428916</v>
+        <v>0.04632659953585609</v>
       </c>
       <c r="E97">
-        <v>0.0005763480051644142</v>
+        <v>0.0005763480051644105</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
@@ -2897,13 +2897,13 @@
         </is>
       </c>
       <c r="C98">
-        <v>-0.30548672296005</v>
+        <v>-0.3054867229600389</v>
       </c>
       <c r="D98">
-        <v>0.04190350079464565</v>
+        <v>0.04190350078934141</v>
       </c>
       <c r="E98">
-        <v>0.0009934630039120751</v>
+        <v>0.0009934630038553481</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -2923,13 +2923,13 @@
         </is>
       </c>
       <c r="C99">
-        <v>-0.4513605322798434</v>
+        <v>-0.4513605322798431</v>
       </c>
       <c r="D99">
-        <v>0.04156990062851939</v>
+        <v>0.04156990062617836</v>
       </c>
       <c r="E99">
-        <v>0.001017955756954909</v>
+        <v>0.001017955756959503</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -2949,13 +2949,13 @@
         </is>
       </c>
       <c r="C100">
-        <v>0.6188485596545492</v>
+        <v>0.618848559654562</v>
       </c>
       <c r="D100">
-        <v>0.04826118478683816</v>
+        <v>0.04826118478869178</v>
       </c>
       <c r="E100">
-        <v>0.0003507650987379716</v>
+        <v>0.0003507650987221592</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -2975,13 +2975,13 @@
         </is>
       </c>
       <c r="C101">
-        <v>3.858134757511312</v>
+        <v>3.858134757511313</v>
       </c>
       <c r="D101">
-        <v>0.02577197744974713</v>
+        <v>0.02577197745129202</v>
       </c>
       <c r="E101">
-        <v>0.0003869448663028779</v>
+        <v>0.0003869448663028746</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -3001,13 +3001,13 @@
         </is>
       </c>
       <c r="C102">
-        <v>1.46775101166588</v>
+        <v>1.467751011665882</v>
       </c>
       <c r="D102">
-        <v>0.0009145016978814393</v>
+        <v>0.0009145016975501846</v>
       </c>
       <c r="E102">
-        <v>1.432838140801309e-06</v>
+        <v>1.432838140903229e-06</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -3027,13 +3027,13 @@
         </is>
       </c>
       <c r="C103">
-        <v>-0.3408493752553961</v>
+        <v>-0.3408493752554012</v>
       </c>
       <c r="D103">
-        <v>0.0331581219298428</v>
+        <v>0.03315812193287432</v>
       </c>
       <c r="E103">
-        <v>0.0005618848551548327</v>
+        <v>0.0005618848551210311</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -3053,13 +3053,13 @@
         </is>
       </c>
       <c r="C104">
-        <v>-0.7682067311205487</v>
+        <v>-0.7682067311205517</v>
       </c>
       <c r="D104">
-        <v>0.03633971621978432</v>
+        <v>0.03633971622202494</v>
       </c>
       <c r="E104">
-        <v>0.0007784385566439445</v>
+        <v>0.0007784385566726917</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -3079,13 +3079,13 @@
         </is>
       </c>
       <c r="C105">
-        <v>-0.5141287239919136</v>
+        <v>-0.5141287239919132</v>
       </c>
       <c r="D105">
-        <v>4.690907004598019e-05</v>
+        <v>4.690907003374811e-05</v>
       </c>
       <c r="E105">
-        <v>2.863193709982848e-08</v>
+        <v>2.863193709645442e-08</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -3105,13 +3105,13 @@
         </is>
       </c>
       <c r="C106">
-        <v>-3.105888275324174</v>
+        <v>-3.105888275324154</v>
       </c>
       <c r="D106">
-        <v>0.02974800126808489</v>
+        <v>0.02974800127151652</v>
       </c>
       <c r="E106">
-        <v>1.66889738763626e-05</v>
+        <v>1.668897387663331e-05</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -3131,13 +3131,13 @@
         </is>
       </c>
       <c r="C107">
-        <v>0.6624135654426996</v>
+        <v>0.6624135654427015</v>
       </c>
       <c r="D107">
-        <v>0.01162913763317422</v>
+        <v>0.01162913763077495</v>
       </c>
       <c r="E107">
-        <v>9.861892378045743e-05</v>
+        <v>9.861892378099627e-05</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
@@ -3157,13 +3157,13 @@
         </is>
       </c>
       <c r="C108">
-        <v>-0.4157445218833076</v>
+        <v>-0.4157445218833088</v>
       </c>
       <c r="D108">
-        <v>0.03926925956023063</v>
+        <v>0.03926925955904021</v>
       </c>
       <c r="E108">
-        <v>0.0008569053627348864</v>
+        <v>0.0008569053627334323</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -3183,13 +3183,13 @@
         </is>
       </c>
       <c r="C109">
-        <v>0.7261306926495457</v>
+        <v>0.7261306926495528</v>
       </c>
       <c r="D109">
-        <v>0.02211292208551394</v>
+        <v>0.02211292208199917</v>
       </c>
       <c r="E109">
-        <v>0.0004381527016483302</v>
+        <v>0.0004381527016588652</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -3209,13 +3209,13 @@
         </is>
       </c>
       <c r="C110">
-        <v>-1.335553206046668</v>
+        <v>-1.335553206046665</v>
       </c>
       <c r="D110">
-        <v>0.03474960898520096</v>
+        <v>0.03474960898356001</v>
       </c>
       <c r="E110">
-        <v>0.0002944774084123096</v>
+        <v>0.0002944774084179582</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -3235,13 +3235,13 @@
         </is>
       </c>
       <c r="C111">
-        <v>-1.212505236786418</v>
+        <v>-1.212505236786422</v>
       </c>
       <c r="D111">
-        <v>0.02353655029410975</v>
+        <v>0.02353655028574947</v>
       </c>
       <c r="E111">
-        <v>0.0002816157915645917</v>
+        <v>0.0002816157915788917</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -3261,13 +3261,13 @@
         </is>
       </c>
       <c r="C112">
-        <v>0.2760633706216135</v>
+        <v>0.2760633706216292</v>
       </c>
       <c r="D112">
-        <v>0.02941351823151872</v>
+        <v>0.02941351822654562</v>
       </c>
       <c r="E112">
-        <v>0.0004776544579996947</v>
+        <v>0.0004776544579479906</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -3287,13 +3287,13 @@
         </is>
       </c>
       <c r="C113">
-        <v>0.3561031967675963</v>
+        <v>0.3561031967675985</v>
       </c>
       <c r="D113">
-        <v>0.03633971621978432</v>
+        <v>0.03633971622202494</v>
       </c>
       <c r="E113">
-        <v>0.0009572131906183784</v>
+        <v>0.0009572131905908057</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -3313,13 +3313,13 @@
         </is>
       </c>
       <c r="C114">
-        <v>-0.3812625226317269</v>
+        <v>-0.3812625226317261</v>
       </c>
       <c r="D114">
-        <v>0.03744843589773193</v>
+        <v>0.0374484358918502</v>
       </c>
       <c r="E114">
-        <v>0.0009942986465645682</v>
+        <v>0.0009942986465505061</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -3339,13 +3339,13 @@
         </is>
       </c>
       <c r="C115">
-        <v>2.786283055468533</v>
+        <v>2.786283055468531</v>
       </c>
       <c r="D115">
-        <v>0.01791268932939229</v>
+        <v>0.01791268933046622</v>
       </c>
       <c r="E115">
-        <v>0.0002046654996843141</v>
+        <v>0.0002046654996843167</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -3365,13 +3365,13 @@
         </is>
       </c>
       <c r="C116">
-        <v>0.5888986194685617</v>
+        <v>0.5888986194685473</v>
       </c>
       <c r="D116">
-        <v>0.01506999081389644</v>
+        <v>0.01506999081437997</v>
       </c>
       <c r="E116">
-        <v>4.350473573469108e-05</v>
+        <v>4.350473573245485e-05</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -3391,13 +3391,13 @@
         </is>
       </c>
       <c r="C117">
-        <v>-0.3016750510943608</v>
+        <v>-0.3016750510943587</v>
       </c>
       <c r="D117">
-        <v>0.03815898390132159</v>
+        <v>0.03815898389959908</v>
       </c>
       <c r="E117">
-        <v>0.001090072120419488</v>
+        <v>0.001090072120370281</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
@@ -3417,13 +3417,13 @@
         </is>
       </c>
       <c r="C118">
-        <v>1.498338402336909</v>
+        <v>1.49833840233693</v>
       </c>
       <c r="D118">
-        <v>0.02420117856227219</v>
+        <v>0.02420117856320418</v>
       </c>
       <c r="E118">
-        <v>0.0001222879986932656</v>
+        <v>0.0001222879986966608</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
@@ -3443,13 +3443,13 @@
         </is>
       </c>
       <c r="C119">
-        <v>1.279043758772736</v>
+        <v>1.279043758772738</v>
       </c>
       <c r="D119">
-        <v>0.005798527488223729</v>
+        <v>0.005798527488752711</v>
       </c>
       <c r="E119">
-        <v>2.56271400692708e-05</v>
+        <v>2.562714007109017e-05</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
@@ -3469,13 +3469,13 @@
         </is>
       </c>
       <c r="C120">
-        <v>-0.6131168956067455</v>
+        <v>-0.6131168956067428</v>
       </c>
       <c r="D120">
-        <v>0.01299851499076815</v>
+        <v>0.01299851499151898</v>
       </c>
       <c r="E120">
-        <v>3.238985718080101e-05</v>
+        <v>3.238985717923535e-05</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -3495,13 +3495,13 @@
         </is>
       </c>
       <c r="C121">
-        <v>1.4831762254002</v>
+        <v>1.483176225400203</v>
       </c>
       <c r="D121">
-        <v>0.03477815041019694</v>
+        <v>0.03477815040807382</v>
       </c>
       <c r="E121">
-        <v>0.000116898017353322</v>
+        <v>0.000116898017353961</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -3521,13 +3521,13 @@
         </is>
       </c>
       <c r="C122">
-        <v>-0.2896488641274119</v>
+        <v>-0.2896488641274114</v>
       </c>
       <c r="D122">
-        <v>0.009644933646618148</v>
+        <v>0.00964493364492354</v>
       </c>
       <c r="E122">
-        <v>8.452875500571003e-05</v>
+        <v>8.452875499600021e-05</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
@@ -3550,7 +3550,7 @@
         <v>2.217048719144076</v>
       </c>
       <c r="D123">
-        <v>0.009981144849153484</v>
+        <v>0.009981144848533874</v>
       </c>
       <c r="E123">
         <v>8.72676537116749e-05</v>
@@ -3573,13 +3573,13 @@
         </is>
       </c>
       <c r="C124">
-        <v>2.68656640219458</v>
+        <v>2.686566402194579</v>
       </c>
       <c r="D124">
-        <v>0.008927151364263648</v>
+        <v>0.008927151364798925</v>
       </c>
       <c r="E124">
-        <v>6.313987682690556e-05</v>
+        <v>6.313987682690604e-05</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
@@ -3599,13 +3599,13 @@
         </is>
       </c>
       <c r="C125">
-        <v>-0.6929074624878326</v>
+        <v>-0.6929074624878323</v>
       </c>
       <c r="D125">
-        <v>0.02523106012644324</v>
+        <v>0.02523106012815507</v>
       </c>
       <c r="E125">
-        <v>0.0003504772208674083</v>
+        <v>0.0003504772208711685</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -3625,13 +3625,13 @@
         </is>
       </c>
       <c r="C126">
-        <v>0.3228517453352397</v>
+        <v>0.3228517453352315</v>
       </c>
       <c r="D126">
-        <v>0.01444076571208121</v>
+        <v>0.01444076571243776</v>
       </c>
       <c r="E126">
-        <v>0.00014788483392782</v>
+        <v>0.0001478848339158777</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
@@ -3651,13 +3651,13 @@
         </is>
       </c>
       <c r="C127">
-        <v>-0.3953865629371456</v>
+        <v>-0.3953865629371435</v>
       </c>
       <c r="D127">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E127">
-        <v>0.0005536326406697467</v>
+        <v>0.0005536326406587209</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
@@ -3677,13 +3677,13 @@
         </is>
       </c>
       <c r="C128">
-        <v>-0.4034218477138531</v>
+        <v>-0.4034218477138551</v>
       </c>
       <c r="D128">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E128">
-        <v>0.0006632689076520232</v>
+        <v>0.0006632689076448029</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -3703,13 +3703,13 @@
         </is>
       </c>
       <c r="C129">
-        <v>-3.210428537725516</v>
+        <v>-3.210428537725508</v>
       </c>
       <c r="D129">
-        <v>0.002009219655518218</v>
+        <v>0.002009219655624703</v>
       </c>
       <c r="E129">
-        <v>2.227918037548768e-07</v>
+        <v>2.227918037513629e-07</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
@@ -3729,13 +3729,13 @@
         </is>
       </c>
       <c r="C130">
-        <v>0.4942358096775014</v>
+        <v>0.4942358096774916</v>
       </c>
       <c r="D130">
-        <v>0.009409867498996999</v>
+        <v>0.009409867499495694</v>
       </c>
       <c r="E130">
-        <v>6.446721476813412e-05</v>
+        <v>6.44672147652721e-05</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
@@ -3755,13 +3755,13 @@
         </is>
       </c>
       <c r="C131">
-        <v>-1.000235229431384</v>
+        <v>-1.000235229431389</v>
       </c>
       <c r="D131">
-        <v>0.0389233265851331</v>
+        <v>0.03892332658774089</v>
       </c>
       <c r="E131">
-        <v>0.0005987804381692128</v>
+        <v>0.000598780438197215</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
@@ -3781,13 +3781,13 @@
         </is>
       </c>
       <c r="C132">
-        <v>-1.20956778849996</v>
+        <v>-1.209567788499963</v>
       </c>
       <c r="D132">
-        <v>0.004828647188975623</v>
+        <v>0.004828647188989144</v>
       </c>
       <c r="E132">
-        <v>2.800491788658491e-05</v>
+        <v>2.800491788836685e-05</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
@@ -3807,13 +3807,13 @@
         </is>
       </c>
       <c r="C133">
-        <v>-0.2835620892259496</v>
+        <v>-0.2835620892259639</v>
       </c>
       <c r="D133">
-        <v>0.04083801840135327</v>
+        <v>0.04083801839987493</v>
       </c>
       <c r="E133">
-        <v>0.0008754604851615645</v>
+        <v>0.0008754604850896587</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
@@ -3833,13 +3833,13 @@
         </is>
       </c>
       <c r="C134">
-        <v>-0.3908345153094576</v>
+        <v>-0.3908345153094623</v>
       </c>
       <c r="D134">
-        <v>0.04083801840135327</v>
+        <v>0.04083801839987493</v>
       </c>
       <c r="E134">
-        <v>0.00090318703046911</v>
+        <v>0.0009031870304566177</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -3859,13 +3859,13 @@
         </is>
       </c>
       <c r="C135">
-        <v>-1.106478518549222</v>
+        <v>-1.106478518549226</v>
       </c>
       <c r="D135">
-        <v>0.03158508029709764</v>
+        <v>0.03158508029852839</v>
       </c>
       <c r="E135">
-        <v>0.000265099667432159</v>
+        <v>0.0002650996674351993</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
@@ -3885,13 +3885,13 @@
         </is>
       </c>
       <c r="C136">
-        <v>-0.3575787855659218</v>
+        <v>-0.3575787855659111</v>
       </c>
       <c r="D136">
-        <v>0.0125379101286632</v>
+        <v>0.01253791012805232</v>
       </c>
       <c r="E136">
-        <v>0.0001492355674673717</v>
+        <v>0.0001492355674601005</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
@@ -3914,10 +3914,10 @@
         <v>2.816999298429498</v>
       </c>
       <c r="D137">
-        <v>0.01346751797729864</v>
+        <v>0.01346751797842208</v>
       </c>
       <c r="E137">
-        <v>3.521947766625002e-05</v>
+        <v>3.521947766624756e-05</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -3937,13 +3937,13 @@
         </is>
       </c>
       <c r="C138">
-        <v>0.4072877540059328</v>
+        <v>0.4072877540058933</v>
       </c>
       <c r="D138">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E138">
-        <v>0.0005129083935666615</v>
+        <v>0.0005129083935305623</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -3963,13 +3963,13 @@
         </is>
       </c>
       <c r="C139">
-        <v>1.368115044003935</v>
+        <v>1.368115044003817</v>
       </c>
       <c r="D139">
-        <v>0.01815898952542409</v>
+        <v>0.01815898952486457</v>
       </c>
       <c r="E139">
-        <v>5.930327736391561e-05</v>
+        <v>5.930327735925535e-05</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -3989,13 +3989,13 @@
         </is>
       </c>
       <c r="C140">
-        <v>-0.6665737782383631</v>
+        <v>-0.6665737782383641</v>
       </c>
       <c r="D140">
-        <v>0.04257024761234196</v>
+        <v>0.04257024760715106</v>
       </c>
       <c r="E140">
-        <v>0.0009382915987587016</v>
+        <v>0.0009382915987793348</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
@@ -4015,13 +4015,13 @@
         </is>
       </c>
       <c r="C141">
-        <v>1.567896224930952</v>
+        <v>1.56789622493097</v>
       </c>
       <c r="D141">
-        <v>0.01557323154892728</v>
+        <v>0.01557323154945418</v>
       </c>
       <c r="E141">
-        <v>4.556738667018253e-05</v>
+        <v>4.556738667236486e-05</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
@@ -4044,7 +4044,7 @@
         <v>3.22645845120462</v>
       </c>
       <c r="D142">
-        <v>0.009644933646618148</v>
+        <v>0.00964493364492354</v>
       </c>
       <c r="E142">
         <v>2.922019225004841e-05</v>
@@ -4067,13 +4067,13 @@
         </is>
       </c>
       <c r="C143">
-        <v>0.4654245597123343</v>
+        <v>0.4654245597123303</v>
       </c>
       <c r="D143">
-        <v>0.03782848334181468</v>
+        <v>0.03782848333505309</v>
       </c>
       <c r="E143">
-        <v>0.0007551268354924314</v>
+        <v>0.0007551268354834568</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
@@ -4093,13 +4093,13 @@
         </is>
       </c>
       <c r="C144">
-        <v>-0.3666293643690056</v>
+        <v>-0.3666293643690075</v>
       </c>
       <c r="D144">
-        <v>0.0456531334999021</v>
+        <v>0.04565313349946096</v>
       </c>
       <c r="E144">
-        <v>0.001492532296274679</v>
+        <v>0.001492532296260256</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -4119,13 +4119,13 @@
         </is>
       </c>
       <c r="C145">
-        <v>-0.4182556786551791</v>
+        <v>-0.4182556786551825</v>
       </c>
       <c r="D145">
-        <v>0.006765880406119975</v>
+        <v>0.006765880404944748</v>
       </c>
       <c r="E145">
-        <v>5.471848987426394e-05</v>
+        <v>5.471848987257972e-05</v>
       </c>
       <c r="F145" t="inlineStr">
         <is>
@@ -4145,13 +4145,13 @@
         </is>
       </c>
       <c r="C146">
-        <v>0.412275382883131</v>
+        <v>0.4122753828831286</v>
       </c>
       <c r="D146">
-        <v>0.04492372637610642</v>
+        <v>0.0449237263759867</v>
       </c>
       <c r="E146">
-        <v>0.001134233351072086</v>
+        <v>0.001134233351061318</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -4171,13 +4171,13 @@
         </is>
       </c>
       <c r="C147">
-        <v>-1.300843003240734</v>
+        <v>-1.300843003240736</v>
       </c>
       <c r="D147">
-        <v>0.0180115130483782</v>
+        <v>0.01801151305034092</v>
       </c>
       <c r="E147">
-        <v>0.0002043239729482212</v>
+        <v>0.0002043239729588161</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -4197,13 +4197,13 @@
         </is>
       </c>
       <c r="C148">
-        <v>-0.2882896912104863</v>
+        <v>-0.2882896912104591</v>
       </c>
       <c r="D148">
-        <v>0.01162913763317422</v>
+        <v>0.01162913763077495</v>
       </c>
       <c r="E148">
-        <v>0.0001068186917158767</v>
+        <v>0.0001068186917012603</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
@@ -4223,13 +4223,13 @@
         </is>
       </c>
       <c r="C149">
-        <v>1.596278381755027</v>
+        <v>1.596278381755025</v>
       </c>
       <c r="D149">
-        <v>0.03633971621978432</v>
+        <v>0.03633971622202494</v>
       </c>
       <c r="E149">
-        <v>0.0001309232983980203</v>
+        <v>0.0001309232983999143</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
@@ -4249,13 +4249,13 @@
         </is>
       </c>
       <c r="C150">
-        <v>-0.3404046329767826</v>
+        <v>-0.3404046329767917</v>
       </c>
       <c r="D150">
-        <v>0.00470179753198625</v>
+        <v>0.004701797531078375</v>
       </c>
       <c r="E150">
-        <v>2.605725690366213e-05</v>
+        <v>2.605725690021575e-05</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
@@ -4275,13 +4275,13 @@
         </is>
       </c>
       <c r="C151">
-        <v>-0.4793103837750768</v>
+        <v>-0.4793103837750781</v>
       </c>
       <c r="D151">
-        <v>0.02242589890201382</v>
+        <v>0.02242589890022221</v>
       </c>
       <c r="E151">
-        <v>0.0003034201245116639</v>
+        <v>0.0003034201245085058</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
@@ -4301,13 +4301,13 @@
         </is>
       </c>
       <c r="C152">
-        <v>-0.4831173352246615</v>
+        <v>-0.483117335224663</v>
       </c>
       <c r="D152">
-        <v>0.03477815041019694</v>
+        <v>0.03477815040807382</v>
       </c>
       <c r="E152">
-        <v>0.0007126887793272905</v>
+        <v>0.0007126887793271349</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -4327,13 +4327,13 @@
         </is>
       </c>
       <c r="C153">
-        <v>2.067757412963037</v>
+        <v>2.067757412963034</v>
       </c>
       <c r="D153">
-        <v>0.02916021884922363</v>
+        <v>0.0291602188519165</v>
       </c>
       <c r="E153">
-        <v>1.61015955899248e-05</v>
+        <v>1.61015955898155e-05</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
@@ -4353,13 +4353,13 @@
         </is>
       </c>
       <c r="C154">
-        <v>2.328030782983395</v>
+        <v>2.328030782983432</v>
       </c>
       <c r="D154">
-        <v>0.009366550973321522</v>
+        <v>0.00936655097171786</v>
       </c>
       <c r="E154">
-        <v>8.841848093589014e-06</v>
+        <v>8.841848094044551e-06</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
@@ -4379,13 +4379,13 @@
         </is>
       </c>
       <c r="C155">
-        <v>-0.3965013451313804</v>
+        <v>-0.3965013451313784</v>
       </c>
       <c r="D155">
-        <v>0.04492372637610642</v>
+        <v>0.0449237263759867</v>
       </c>
       <c r="E155">
-        <v>0.0007741720063312605</v>
+        <v>0.000774172006316681</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
@@ -4408,7 +4408,7 @@
         <v>3.47756372365238</v>
       </c>
       <c r="D156">
-        <v>0.003248468294483337</v>
+        <v>0.003248468294584027</v>
       </c>
       <c r="E156">
         <v>6.313669399258746e-06</v>
@@ -4434,7 +4434,7 @@
         <v>3.322311344183442</v>
       </c>
       <c r="D157">
-        <v>0.03782848334181468</v>
+        <v>0.03782848333505309</v>
       </c>
       <c r="E157">
         <v>0.0002093496484891562</v>
@@ -4457,13 +4457,13 @@
         </is>
       </c>
       <c r="C158">
-        <v>-0.3469650158918686</v>
+        <v>-0.3469650158918707</v>
       </c>
       <c r="D158">
-        <v>0.01741509362642408</v>
+        <v>0.0174150936232065</v>
       </c>
       <c r="E158">
-        <v>0.0002497972102847089</v>
+        <v>0.0002497972102742576</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
@@ -4483,13 +4483,13 @@
         </is>
       </c>
       <c r="C159">
-        <v>-0.3408394361773102</v>
+        <v>-0.3408394361773051</v>
       </c>
       <c r="D159">
-        <v>0.0268475521853169</v>
+        <v>0.02684755218341859</v>
       </c>
       <c r="E159">
-        <v>0.0003926763994783359</v>
+        <v>0.0003926763994618084</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
@@ -4509,13 +4509,13 @@
         </is>
       </c>
       <c r="C160">
-        <v>-0.7436045914685921</v>
+        <v>-0.7436045914685925</v>
       </c>
       <c r="D160">
-        <v>7.588970384797442e-06</v>
+        <v>7.588970384693581e-06</v>
       </c>
       <c r="E160">
-        <v>3.613183665367611e-09</v>
+        <v>3.613183665318159e-09</v>
       </c>
       <c r="F160" t="inlineStr">
         <is>
@@ -4535,13 +4535,13 @@
         </is>
       </c>
       <c r="C161">
-        <v>-0.4365735859959936</v>
+        <v>-0.4365735859959962</v>
       </c>
       <c r="D161">
-        <v>0.002443122730665308</v>
+        <v>0.002443122730705648</v>
       </c>
       <c r="E161">
-        <v>1.220237075996692e-05</v>
+        <v>1.220237075947784e-05</v>
       </c>
       <c r="F161" t="inlineStr">
         <is>
@@ -4561,13 +4561,13 @@
         </is>
       </c>
       <c r="C162">
-        <v>1.695135492302047</v>
+        <v>1.695135492302066</v>
       </c>
       <c r="D162">
-        <v>0.01060929420368479</v>
+        <v>0.01060929420343393</v>
       </c>
       <c r="E162">
-        <v>2.371473689196683e-05</v>
+        <v>2.371473689263349e-05</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
@@ -4587,13 +4587,13 @@
         </is>
       </c>
       <c r="C163">
-        <v>-0.7351454973211333</v>
+        <v>-0.7351454973211342</v>
       </c>
       <c r="D163">
-        <v>0.03474960898520096</v>
+        <v>0.03474960898356001</v>
       </c>
       <c r="E163">
-        <v>0.0002273266355080298</v>
+        <v>0.000227326635495036</v>
       </c>
       <c r="F163" t="inlineStr">
         <is>
@@ -4613,13 +4613,13 @@
         </is>
       </c>
       <c r="C164">
-        <v>1.25844450581611</v>
+        <v>1.258444505816111</v>
       </c>
       <c r="D164">
-        <v>0.002394751672761807</v>
+        <v>0.002394751672878058</v>
       </c>
       <c r="E164">
-        <v>8.474033174186229e-06</v>
+        <v>8.4740331748401e-06</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
@@ -4639,13 +4639,13 @@
         </is>
       </c>
       <c r="C165">
-        <v>-0.2725497014833948</v>
+        <v>-0.2725497014833981</v>
       </c>
       <c r="D165">
-        <v>0.03782848334181468</v>
+        <v>0.03782848333505309</v>
       </c>
       <c r="E165">
-        <v>0.0007877648003393575</v>
+        <v>0.0007877648002849584</v>
       </c>
       <c r="F165" t="inlineStr">
         <is>
@@ -4665,13 +4665,13 @@
         </is>
       </c>
       <c r="C166">
-        <v>-0.7242825220118112</v>
+        <v>-0.7242825220118108</v>
       </c>
       <c r="D166">
-        <v>0.02242589890201382</v>
+        <v>0.02242589890022221</v>
       </c>
       <c r="E166">
-        <v>0.0002937074245361906</v>
+        <v>0.0002937074245399053</v>
       </c>
       <c r="F166" t="inlineStr">
         <is>
@@ -4691,13 +4691,13 @@
         </is>
       </c>
       <c r="C167">
-        <v>-0.3944236043809516</v>
+        <v>-0.3944236043809543</v>
       </c>
       <c r="D167">
-        <v>0.04546639834046843</v>
+        <v>0.0454663983337168</v>
       </c>
       <c r="E167">
-        <v>0.001422257819829007</v>
+        <v>0.001422257819821073</v>
       </c>
       <c r="F167" t="inlineStr">
         <is>
@@ -4717,10 +4717,10 @@
         </is>
       </c>
       <c r="C168">
-        <v>5.280249149498188</v>
+        <v>5.280249149498189</v>
       </c>
       <c r="D168">
-        <v>0.0008689191171967279</v>
+        <v>0.0008689191171020561</v>
       </c>
       <c r="E168">
         <v>1.084235102682439e-06</v>
@@ -4743,13 +4743,13 @@
         </is>
       </c>
       <c r="C169">
-        <v>-0.7423874041755367</v>
+        <v>-0.7423874041755411</v>
       </c>
       <c r="D169">
-        <v>0.003290474777808043</v>
+        <v>0.003290474778190419</v>
       </c>
       <c r="E169">
-        <v>1.803607808853224e-05</v>
+        <v>1.803607808899655e-05</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
@@ -4769,13 +4769,13 @@
         </is>
       </c>
       <c r="C170">
-        <v>-0.6600416883645186</v>
+        <v>-0.6600416883645207</v>
       </c>
       <c r="D170">
-        <v>0.000544958633238181</v>
+        <v>0.0005449586332023876</v>
       </c>
       <c r="E170">
-        <v>6.321241199922281e-07</v>
+        <v>6.32124119989161e-07</v>
       </c>
       <c r="F170" t="inlineStr">
         <is>
@@ -4795,13 +4795,13 @@
         </is>
       </c>
       <c r="C171">
-        <v>-2.397517316288367</v>
+        <v>-2.397517316288366</v>
       </c>
       <c r="D171">
-        <v>0.03277896192965388</v>
+        <v>0.03277896193031708</v>
       </c>
       <c r="E171">
-        <v>0.0005801399619292806</v>
+        <v>0.0005801399619292853</v>
       </c>
       <c r="F171" t="inlineStr">
         <is>
@@ -4824,7 +4824,7 @@
         <v>-7.015542953881988</v>
       </c>
       <c r="D172">
-        <v>0.002475457323386624</v>
+        <v>0.002475457323673573</v>
       </c>
       <c r="E172">
         <v>2.662464628553274e-06</v>
@@ -4847,13 +4847,13 @@
         </is>
       </c>
       <c r="C173">
-        <v>0.6688633984539529</v>
+        <v>0.6688633984539518</v>
       </c>
       <c r="D173">
-        <v>0.009673264429536668</v>
+        <v>0.009673264429135452</v>
       </c>
       <c r="E173">
-        <v>3.97310676500951e-05</v>
+        <v>3.973106764710308e-05</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
@@ -4873,13 +4873,13 @@
         </is>
       </c>
       <c r="C174">
-        <v>-0.3679593995787733</v>
+        <v>-0.3679593995787731</v>
       </c>
       <c r="D174">
-        <v>0.00470179753198625</v>
+        <v>0.004701797531078375</v>
       </c>
       <c r="E174">
-        <v>2.266427753036788e-05</v>
+        <v>2.266427752853952e-05</v>
       </c>
       <c r="F174" t="inlineStr">
         <is>
@@ -4899,13 +4899,13 @@
         </is>
       </c>
       <c r="C175">
-        <v>0.6616392960129371</v>
+        <v>0.6616392960129392</v>
       </c>
       <c r="D175">
-        <v>0.04580293991767476</v>
+        <v>0.04580293991243103</v>
       </c>
       <c r="E175">
-        <v>0.001453752940701674</v>
+        <v>0.001453752940743011</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -4925,13 +4925,13 @@
         </is>
       </c>
       <c r="C176">
-        <v>1.046078690049057</v>
+        <v>1.046078690049041</v>
       </c>
       <c r="D176">
-        <v>0.02289688514022564</v>
+        <v>0.02289688513790355</v>
       </c>
       <c r="E176">
-        <v>0.0001759411181511345</v>
+        <v>0.0001759411181573796</v>
       </c>
       <c r="F176" t="inlineStr">
         <is>
@@ -4951,13 +4951,13 @@
         </is>
       </c>
       <c r="C177">
-        <v>-0.4687912218656147</v>
+        <v>-0.4687912218656142</v>
       </c>
       <c r="D177">
-        <v>0.03633971621978432</v>
+        <v>0.03633971622202494</v>
       </c>
       <c r="E177">
-        <v>0.0008683423033967085</v>
+        <v>0.0008683423033984633</v>
       </c>
       <c r="F177" t="inlineStr">
         <is>
@@ -4977,13 +4977,13 @@
         </is>
       </c>
       <c r="C178">
-        <v>-0.3775815064574771</v>
+        <v>-0.3775815064574731</v>
       </c>
       <c r="D178">
-        <v>0.0233185286883232</v>
+        <v>0.02331852868599866</v>
       </c>
       <c r="E178">
-        <v>0.0003241807267893068</v>
+        <v>0.0003241807267795153</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -5003,13 +5003,13 @@
         </is>
       </c>
       <c r="C179">
-        <v>-0.3982893689825124</v>
+        <v>-0.3982893689825153</v>
       </c>
       <c r="D179">
-        <v>0.02211292208551394</v>
+        <v>0.02211292208199917</v>
       </c>
       <c r="E179">
-        <v>0.0003610470742539831</v>
+        <v>0.0003610470742481964</v>
       </c>
       <c r="F179" t="inlineStr">
         <is>
@@ -5029,13 +5029,13 @@
         </is>
       </c>
       <c r="C180">
-        <v>1.817137857669314</v>
+        <v>1.817137857669324</v>
       </c>
       <c r="D180">
-        <v>0.02353655029410975</v>
+        <v>0.02353655028574947</v>
       </c>
       <c r="E180">
-        <v>9.157674204010924e-05</v>
+        <v>9.157674204153789e-05</v>
       </c>
       <c r="F180" t="inlineStr">
         <is>
@@ -5055,13 +5055,13 @@
         </is>
       </c>
       <c r="C181">
-        <v>-0.2907483741436849</v>
+        <v>-0.2907483741436895</v>
       </c>
       <c r="D181">
-        <v>0.0195286484946758</v>
+        <v>0.01952864849493564</v>
       </c>
       <c r="E181">
-        <v>0.0002356030032319173</v>
+        <v>0.0002356030032100246</v>
       </c>
       <c r="F181" t="inlineStr">
         <is>
@@ -5084,10 +5084,10 @@
         <v>-1.007330774160721</v>
       </c>
       <c r="D182">
-        <v>0.04257024761234196</v>
+        <v>0.04257024760715106</v>
       </c>
       <c r="E182">
-        <v>0.0004574001242036507</v>
+        <v>0.0004574001242044342</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -5107,13 +5107,13 @@
         </is>
       </c>
       <c r="C183">
-        <v>-4.248675433928231</v>
+        <v>-4.248675433928228</v>
       </c>
       <c r="D183">
-        <v>0.01557323154892728</v>
+        <v>0.01557323154945418</v>
       </c>
       <c r="E183">
-        <v>8.343136236027412e-05</v>
+        <v>8.343136236027442e-05</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
@@ -5133,13 +5133,13 @@
         </is>
       </c>
       <c r="C184">
-        <v>0.9804557433245307</v>
+        <v>0.9804557433245301</v>
       </c>
       <c r="D184">
-        <v>0.0195286484946758</v>
+        <v>0.01952864849493564</v>
       </c>
       <c r="E184">
-        <v>8.771361041881218e-05</v>
+        <v>8.771361041903665e-05</v>
       </c>
       <c r="F184" t="inlineStr">
         <is>
@@ -5159,13 +5159,13 @@
         </is>
       </c>
       <c r="C185">
-        <v>2.095991410146141</v>
+        <v>2.095991410146163</v>
       </c>
       <c r="D185">
-        <v>0.008779509299463266</v>
+        <v>0.008779509299270207</v>
       </c>
       <c r="E185">
-        <v>1.499105694943521e-05</v>
+        <v>1.499105694988145e-05</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
@@ -5185,13 +5185,13 @@
         </is>
       </c>
       <c r="C186">
-        <v>2.137166671871327</v>
+        <v>2.137166671871328</v>
       </c>
       <c r="D186">
-        <v>0.03477815041019694</v>
+        <v>0.03477815040807382</v>
       </c>
       <c r="E186">
-        <v>0.0007071581649123885</v>
+        <v>0.0007071581649123838</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -5211,13 +5211,13 @@
         </is>
       </c>
       <c r="C187">
-        <v>-0.4112802965966424</v>
+        <v>-0.4112802965966441</v>
       </c>
       <c r="D187">
-        <v>0.01408956698523881</v>
+        <v>0.01408956698401284</v>
       </c>
       <c r="E187">
-        <v>0.0001416408630541553</v>
+        <v>0.0001416408630504466</v>
       </c>
       <c r="F187" t="inlineStr">
         <is>
@@ -5237,13 +5237,13 @@
         </is>
       </c>
       <c r="C188">
-        <v>0.9273840692554657</v>
+        <v>0.927384069255466</v>
       </c>
       <c r="D188">
-        <v>0.0331581219298428</v>
+        <v>0.03315812193287432</v>
       </c>
       <c r="E188">
-        <v>0.000613044737589071</v>
+        <v>0.0006130447376083655</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -5263,13 +5263,13 @@
         </is>
       </c>
       <c r="C189">
-        <v>2.102881237092276</v>
+        <v>2.102881237092279</v>
       </c>
       <c r="D189">
-        <v>0.001726430185562854</v>
+        <v>0.001726430185642135</v>
       </c>
       <c r="E189">
-        <v>2.17848638200378e-06</v>
+        <v>2.17848638212735e-06</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
@@ -5289,13 +5289,13 @@
         </is>
       </c>
       <c r="C190">
-        <v>1.15256381075752</v>
+        <v>1.152563810757513</v>
       </c>
       <c r="D190">
-        <v>0.001295299920993254</v>
+        <v>0.001295299921131314</v>
       </c>
       <c r="E190">
-        <v>3.13416697444882e-06</v>
+        <v>3.134166974616822e-06</v>
       </c>
       <c r="F190" t="inlineStr">
         <is>
@@ -5315,13 +5315,13 @@
         </is>
       </c>
       <c r="C191">
-        <v>-0.4693569324656254</v>
+        <v>-0.4693569324656271</v>
       </c>
       <c r="D191">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E191">
-        <v>0.0006551919593826431</v>
+        <v>0.0006551919593865334</v>
       </c>
       <c r="F191" t="inlineStr">
         <is>
@@ -5341,13 +5341,13 @@
         </is>
       </c>
       <c r="C192">
-        <v>3.208131522693819</v>
+        <v>3.208131522693821</v>
       </c>
       <c r="D192">
-        <v>0.01661820551864299</v>
+        <v>0.01661820551898432</v>
       </c>
       <c r="E192">
-        <v>8.358066370196902e-05</v>
+        <v>8.358066370196826e-05</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -5367,13 +5367,13 @@
         </is>
       </c>
       <c r="C193">
-        <v>4.687161658924638</v>
+        <v>4.687161658924641</v>
       </c>
       <c r="D193">
-        <v>0.001726430185562854</v>
+        <v>0.001726430185642135</v>
       </c>
       <c r="E193">
-        <v>4.330975633600614e-06</v>
+        <v>4.330975633600558e-06</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -5393,13 +5393,13 @@
         </is>
       </c>
       <c r="C194">
-        <v>0.896557289442975</v>
+        <v>0.896557289442971</v>
       </c>
       <c r="D194">
-        <v>0.005625838982361868</v>
+        <v>0.005625838981755759</v>
       </c>
       <c r="E194">
-        <v>3.192858383182252e-05</v>
+        <v>3.192858383347126e-05</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
@@ -5419,13 +5419,13 @@
         </is>
       </c>
       <c r="C195">
-        <v>0.7761475791155124</v>
+        <v>0.7761475791155071</v>
       </c>
       <c r="D195">
-        <v>0.04412449928642177</v>
+        <v>0.04412449928013371</v>
       </c>
       <c r="E195">
-        <v>0.001062587904085065</v>
+        <v>0.00106258790410635</v>
       </c>
       <c r="F195" t="inlineStr">
         <is>
@@ -5445,10 +5445,10 @@
         </is>
       </c>
       <c r="C196">
-        <v>3.273759088560353</v>
+        <v>3.273759088560354</v>
       </c>
       <c r="D196">
-        <v>0.00470179753198625</v>
+        <v>0.004701797531078375</v>
       </c>
       <c r="E196">
         <v>2.247724631018127e-05</v>
@@ -5471,13 +5471,13 @@
         </is>
       </c>
       <c r="C197">
-        <v>4.458856104011831</v>
+        <v>4.458856104011833</v>
       </c>
       <c r="D197">
-        <v>0.001295299920993254</v>
+        <v>0.001295299921131314</v>
       </c>
       <c r="E197">
-        <v>3.957282312497549e-06</v>
+        <v>3.957282312497515e-06</v>
       </c>
       <c r="F197" t="inlineStr">
         <is>
@@ -5497,13 +5497,13 @@
         </is>
       </c>
       <c r="C198">
-        <v>2.449694358766036</v>
+        <v>2.449694358766037</v>
       </c>
       <c r="D198">
-        <v>0.03477815041019694</v>
+        <v>0.03477815040807382</v>
       </c>
       <c r="E198">
-        <v>0.0003020473570164628</v>
+        <v>0.0003020473570164593</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
@@ -5523,13 +5523,13 @@
         </is>
       </c>
       <c r="C199">
-        <v>-0.4509671898583348</v>
+        <v>-0.4509671898583334</v>
       </c>
       <c r="D199">
-        <v>0.004592942540983284</v>
+        <v>0.004592942540438952</v>
       </c>
       <c r="E199">
-        <v>2.223430934266481e-05</v>
+        <v>2.22343093415746e-05</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
@@ -5549,13 +5549,13 @@
         </is>
       </c>
       <c r="C200">
-        <v>-1.776297270601188</v>
+        <v>-1.776297270601177</v>
       </c>
       <c r="D200">
-        <v>0.0305058511316976</v>
+        <v>0.03050585113136554</v>
       </c>
       <c r="E200">
-        <v>8.6664821075856e-05</v>
+        <v>8.666482107791102e-05</v>
       </c>
       <c r="F200" t="inlineStr">
         <is>
@@ -5575,13 +5575,13 @@
         </is>
       </c>
       <c r="C201">
-        <v>4.403195032825925</v>
+        <v>4.403195032825927</v>
       </c>
       <c r="D201">
-        <v>0.01763574010417309</v>
+        <v>0.01763574010326006</v>
       </c>
       <c r="E201">
-        <v>5.201356445039111e-05</v>
+        <v>5.201356445039032e-05</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -5601,13 +5601,13 @@
         </is>
       </c>
       <c r="C202">
-        <v>-0.6110971568144096</v>
+        <v>-0.6110971568144055</v>
       </c>
       <c r="D202">
-        <v>0.005625838982361868</v>
+        <v>0.005625838981755759</v>
       </c>
       <c r="E202">
-        <v>3.222186947580792e-05</v>
+        <v>3.222186947452172e-05</v>
       </c>
       <c r="F202" t="inlineStr">
         <is>
@@ -5627,13 +5627,13 @@
         </is>
       </c>
       <c r="C203">
-        <v>-0.3772518551120936</v>
+        <v>-0.377251855112089</v>
       </c>
       <c r="D203">
-        <v>0.01557323154892728</v>
+        <v>0.01557323154945418</v>
       </c>
       <c r="E203">
-        <v>0.0002090685200071603</v>
+        <v>0.0002090685199965939</v>
       </c>
       <c r="F203" t="inlineStr">
         <is>
@@ -5653,13 +5653,13 @@
         </is>
       </c>
       <c r="C204">
-        <v>-0.8899647675100677</v>
+        <v>-0.8899647675100646</v>
       </c>
       <c r="D204">
-        <v>0.002144929856903135</v>
+        <v>0.00214492985706972</v>
       </c>
       <c r="E204">
-        <v>1.966896376773647e-06</v>
+        <v>1.966896376762195e-06</v>
       </c>
       <c r="F204" t="inlineStr">
         <is>
@@ -5679,13 +5679,13 @@
         </is>
       </c>
       <c r="C205">
-        <v>-0.4881954958730174</v>
+        <v>-0.4881954958730092</v>
       </c>
       <c r="D205">
-        <v>0.009525611148362237</v>
+        <v>0.009525611148482353</v>
       </c>
       <c r="E205">
-        <v>6.645782103400153e-05</v>
+        <v>6.645782103159692e-05</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -5705,13 +5705,13 @@
         </is>
       </c>
       <c r="C206">
-        <v>1.167326972083206</v>
+        <v>1.167326972083203</v>
       </c>
       <c r="D206">
-        <v>0.0009196851532549835</v>
+        <v>0.0009196851533286504</v>
       </c>
       <c r="E206">
-        <v>5.622329606375361e-07</v>
+        <v>5.622329606356313e-07</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
@@ -5731,13 +5731,13 @@
         </is>
       </c>
       <c r="C207">
-        <v>-0.6630318669611848</v>
+        <v>-0.663031866961184</v>
       </c>
       <c r="D207">
-        <v>0.03488258415377721</v>
+        <v>0.03488258414835176</v>
       </c>
       <c r="E207">
-        <v>0.000183800955336297</v>
+        <v>0.0001838009553335843</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
@@ -5757,13 +5757,13 @@
         </is>
       </c>
       <c r="C208">
-        <v>-0.3409992633256098</v>
+        <v>-0.3409992633256138</v>
       </c>
       <c r="D208">
-        <v>0.04492372637610642</v>
+        <v>0.0449237263759867</v>
       </c>
       <c r="E208">
-        <v>0.001132216512047201</v>
+        <v>0.001132216512025989</v>
       </c>
       <c r="F208" t="inlineStr">
         <is>
@@ -5783,13 +5783,13 @@
         </is>
       </c>
       <c r="C209">
-        <v>-0.6309395807521745</v>
+        <v>-0.630939580752177</v>
       </c>
       <c r="D209">
-        <v>0.002443122730665308</v>
+        <v>0.002443122730705648</v>
       </c>
       <c r="E209">
-        <v>1.240741155697817e-05</v>
+        <v>1.240741155718302e-05</v>
       </c>
       <c r="F209" t="inlineStr">
         <is>
@@ -5809,13 +5809,13 @@
         </is>
       </c>
       <c r="C210">
-        <v>-0.3731636487316148</v>
+        <v>-0.3731636487316163</v>
       </c>
       <c r="D210">
-        <v>0.04083801840135327</v>
+        <v>0.04083801839987493</v>
       </c>
       <c r="E210">
-        <v>0.000901699836573801</v>
+        <v>0.0009016998365603312</v>
       </c>
       <c r="F210" t="inlineStr">
         <is>
@@ -5835,13 +5835,13 @@
         </is>
       </c>
       <c r="C211">
-        <v>1.459191505035934</v>
+        <v>1.459191505035938</v>
       </c>
       <c r="D211">
-        <v>0.01506999081389644</v>
+        <v>0.01506999081437997</v>
       </c>
       <c r="E211">
-        <v>4.234402292700459e-05</v>
+        <v>4.234402292876804e-05</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -5861,13 +5861,13 @@
         </is>
       </c>
       <c r="C212">
-        <v>0.8717460950949064</v>
+        <v>0.871746095094921</v>
       </c>
       <c r="D212">
-        <v>0.0189210820647947</v>
+        <v>0.01892108206508711</v>
       </c>
       <c r="E212">
-        <v>0.0001050705800869126</v>
+        <v>0.0001050705800852797</v>
       </c>
       <c r="F212" t="inlineStr">
         <is>
@@ -5887,13 +5887,13 @@
         </is>
       </c>
       <c r="C213">
-        <v>-0.5702160728667967</v>
+        <v>-0.5702160728667963</v>
       </c>
       <c r="D213">
-        <v>0.04492372637610642</v>
+        <v>0.0449237263759867</v>
       </c>
       <c r="E213">
-        <v>0.001127106402430383</v>
+        <v>0.001127106402440281</v>
       </c>
       <c r="F213" t="inlineStr">
         <is>
@@ -5913,13 +5913,13 @@
         </is>
       </c>
       <c r="C214">
-        <v>1.859114756883011</v>
+        <v>1.85911475688302</v>
       </c>
       <c r="D214">
-        <v>0.008796238015231578</v>
+        <v>0.008796238015391764</v>
       </c>
       <c r="E214">
-        <v>1.031624434373348e-05</v>
+        <v>1.031624434389323e-05</v>
       </c>
       <c r="F214" t="inlineStr">
         <is>
@@ -5939,13 +5939,13 @@
         </is>
       </c>
       <c r="C215">
-        <v>1.331250980100857</v>
+        <v>1.331250980100859</v>
       </c>
       <c r="D215">
-        <v>0.01549569644597233</v>
+        <v>0.01549569644593907</v>
       </c>
       <c r="E215">
-        <v>2.790912186816619e-05</v>
+        <v>2.790912186803019e-05</v>
       </c>
       <c r="F215" t="inlineStr">
         <is>

</xml_diff>